<commit_message>
Add field to manage task
</commit_message>
<xml_diff>
--- a/data/goals_and_tasks.xlsx
+++ b/data/goals_and_tasks.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t>Goal ID</t>
   </si>
@@ -27,7 +27,7 @@
     <t>Target Date</t>
   </si>
   <si>
-    <t>573cbff9-baa8-4ec9-813d-887793889e66</t>
+    <t>f9711b89-3ce0-4bfd-a04f-6f81b5d022bf</t>
   </si>
   <si>
     <t>Learn Java</t>
@@ -39,7 +39,7 @@
     <t>2024-12-31</t>
   </si>
   <si>
-    <t>4b785da4-8182-4b87-8915-67f0d8f0e2dc</t>
+    <t>4c1c63fe-4a4c-4fd4-8745-50e98558f9e3</t>
   </si>
   <si>
     <t>Improve UI Design</t>
@@ -51,7 +51,7 @@
     <t>2025-08-15</t>
   </si>
   <si>
-    <t>b8ca06b8-639a-411b-99fb-95dcc3c29a44</t>
+    <t>b479bde7-6297-4452-93c9-e634029b6316</t>
   </si>
   <si>
     <t>Learn Spring Boot</t>
@@ -60,7 +60,7 @@
     <t>2025-12-31</t>
   </si>
   <si>
-    <t>f2d05909-6da7-4a59-85ad-5e3ff780ba74</t>
+    <t>1f4f0d7f-ba7b-49b0-ae1d-7edfda512c48</t>
   </si>
   <si>
     <t>Learn English</t>
@@ -87,9 +87,27 @@
     <t>Task Due Date</t>
   </si>
   <si>
+    <t>Task Status</t>
+  </si>
+  <si>
     <t>Task Completed</t>
   </si>
   <si>
+    <t>5258a021-56cd-4f68-8ef5-386e86136170</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Improve code 2</t>
+  </si>
+  <si>
+    <t>URGENT</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
     <t>246b36ce-0da3-49d5-8857-21e915cc6156</t>
   </si>
   <si>
@@ -105,13 +123,52 @@
     <t>2025-07-31</t>
   </si>
   <si>
-    <t>5258a021-56cd-4f68-8ef5-386e86136170</t>
-  </si>
-  <si>
-    <t>Test 2</t>
-  </si>
-  <si>
-    <t>Improve code 2</t>
+    <t>f1aa0ec7-7cb9-425a-aea9-63c6ae02f69b</t>
+  </si>
+  <si>
+    <t>Test 5</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2025-07-22</t>
+  </si>
+  <si>
+    <t>To Do</t>
+  </si>
+  <si>
+    <t>aa303491-34d2-4288-a7de-a1f6447ec458</t>
+  </si>
+  <si>
+    <t>Read and understand the first chapter</t>
+  </si>
+  <si>
+    <t>2024-07-31</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>fd6629f6-fa17-4f85-8535-415c81b82152</t>
+  </si>
+  <si>
+    <t>Read and understand the second chapter</t>
+  </si>
+  <si>
+    <t>2024-08-09</t>
+  </si>
+  <si>
+    <t>60253cbd-d36b-42ec-be9b-331b0d225447</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Improve code 1</t>
+  </si>
+  <si>
+    <t>2025-07-08</t>
   </si>
   <si>
     <t>fa838930-1316-42a7-8f8f-28d675abfa9c</t>
@@ -123,70 +180,25 @@
     <t>Improve code 3</t>
   </si>
   <si>
-    <t>2025-07-10</t>
-  </si>
-  <si>
-    <t>f1aa0ec7-7cb9-425a-aea9-63c6ae02f69b</t>
-  </si>
-  <si>
-    <t>Test 5</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>2025-07-22</t>
-  </si>
-  <si>
-    <t>60253cbd-d36b-42ec-be9b-331b0d225447</t>
-  </si>
-  <si>
-    <t>Test 1</t>
-  </si>
-  <si>
-    <t>Improve code 1</t>
-  </si>
-  <si>
-    <t>2025-07-08</t>
-  </si>
-  <si>
-    <t>fd6629f6-fa17-4f85-8535-415c81b82152</t>
-  </si>
-  <si>
-    <t>Read and understand the second chapter</t>
+    <t>2025-08-08</t>
+  </si>
+  <si>
+    <t>b60a251c-299a-4d3d-97bb-7efca4f88f97</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>2025-07-23</t>
+  </si>
+  <si>
+    <t>45008821-c270-42fc-9a00-e93c53c9d14c</t>
+  </si>
+  <si>
+    <t>Improve Code</t>
   </si>
   <si>
     <t>HIGH</t>
-  </si>
-  <si>
-    <t>2024-07-15</t>
-  </si>
-  <si>
-    <t>aa303491-34d2-4288-a7de-a1f6447ec458</t>
-  </si>
-  <si>
-    <t>Read and understand the first chapter</t>
-  </si>
-  <si>
-    <t>URGENT</t>
-  </si>
-  <si>
-    <t>2024-06-27</t>
-  </si>
-  <si>
-    <t>b60a251c-299a-4d3d-97bb-7efca4f88f97</t>
-  </si>
-  <si>
-    <t>Coding</t>
-  </si>
-  <si>
-    <t>2025-07-23</t>
-  </si>
-  <si>
-    <t>45008821-c270-42fc-9a00-e93c53c9d14c</t>
-  </si>
-  <si>
-    <t>Improve Code</t>
   </si>
 </sst>
 </file>
@@ -314,7 +326,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -342,211 +354,241 @@
       <c r="G1" t="s" s="0">
         <v>24</v>
       </c>
+      <c r="H1" t="s" s="0">
+        <v>25</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="G2" t="b" s="0">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="H2" t="b" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="G3" t="b" s="0">
+      <c r="H3" t="b" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C4" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="D4" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>28</v>
-      </c>
       <c r="F4" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="G4" t="b" s="0">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H4" t="b" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="G5" t="b" s="0">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="H5" t="b" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="G6" t="b" s="0">
-        <v>0</v>
+      <c r="H6" t="b" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="G7" t="b" s="0">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="H7" t="b" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="G8" t="b" s="0">
+        <v>55</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="H8" t="b" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s" s="0">
         <v>9</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s" s="0">
         <v>9</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="G9" t="b" s="0">
+        <v>58</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H9" t="b" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s" s="0">
         <v>13</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s" s="0">
         <v>13</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="G10" t="b" s="0">
+        <v>58</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H10" t="b" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve UI of View Goals and Tasks
</commit_message>
<xml_diff>
--- a/data/goals_and_tasks.xlsx
+++ b/data/goals_and_tasks.xlsx
@@ -27,7 +27,31 @@
     <t>Target Date</t>
   </si>
   <si>
-    <t>f9711b89-3ce0-4bfd-a04f-6f81b5d022bf</t>
+    <t>6b686207-ba2e-4ed4-96e1-95e467721ddf</t>
+  </si>
+  <si>
+    <t>Learn English</t>
+  </si>
+  <si>
+    <t>MONTHLY</t>
+  </si>
+  <si>
+    <t>2025-07-24</t>
+  </si>
+  <si>
+    <t>ab0802b0-a7b8-4f8d-870d-cf2abf2e64d0</t>
+  </si>
+  <si>
+    <t>Improve UI Design</t>
+  </si>
+  <si>
+    <t>SHORT_TERM</t>
+  </si>
+  <si>
+    <t>2025-08-15</t>
+  </si>
+  <si>
+    <t>17d8a0b5-7c59-4965-929f-0858c56197a5</t>
   </si>
   <si>
     <t>Learn Java</t>
@@ -39,19 +63,7 @@
     <t>2024-12-31</t>
   </si>
   <si>
-    <t>4c1c63fe-4a4c-4fd4-8745-50e98558f9e3</t>
-  </si>
-  <si>
-    <t>Improve UI Design</t>
-  </si>
-  <si>
-    <t>SHORT_TERM</t>
-  </si>
-  <si>
-    <t>2025-08-15</t>
-  </si>
-  <si>
-    <t>b479bde7-6297-4452-93c9-e634029b6316</t>
+    <t>4cfaf309-4c63-4357-8f9d-afe2dc57dc51</t>
   </si>
   <si>
     <t>Learn Spring Boot</t>
@@ -60,18 +72,6 @@
     <t>2025-12-31</t>
   </si>
   <si>
-    <t>1f4f0d7f-ba7b-49b0-ae1d-7edfda512c48</t>
-  </si>
-  <si>
-    <t>Learn English</t>
-  </si>
-  <si>
-    <t>MONTHLY</t>
-  </si>
-  <si>
-    <t>2025-07-24</t>
-  </si>
-  <si>
     <t>Task ID</t>
   </si>
   <si>
@@ -93,6 +93,21 @@
     <t>Task Completed</t>
   </si>
   <si>
+    <t>b60a251c-299a-4d3d-97bb-7efca4f88f97</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>2025-07-23</t>
+  </si>
+  <si>
+    <t>To Do</t>
+  </si>
+  <si>
     <t>5258a021-56cd-4f68-8ef5-386e86136170</t>
   </si>
   <si>
@@ -102,48 +117,45 @@
     <t>Improve code 2</t>
   </si>
   <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>246b36ce-0da3-49d5-8857-21e915cc6156</t>
+  </si>
+  <si>
+    <t>Learn Java sprint 1</t>
+  </si>
+  <si>
+    <t>Understand logic</t>
+  </si>
+  <si>
+    <t>2025-07-31</t>
+  </si>
+  <si>
+    <t>f1aa0ec7-7cb9-425a-aea9-63c6ae02f69b</t>
+  </si>
+  <si>
+    <t>Test 5</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2025-07-22</t>
+  </si>
+  <si>
+    <t>aa303491-34d2-4288-a7de-a1f6447ec458</t>
+  </si>
+  <si>
+    <t>Read and understand the first chapter</t>
+  </si>
+  <si>
     <t>URGENT</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>246b36ce-0da3-49d5-8857-21e915cc6156</t>
-  </si>
-  <si>
-    <t>Learn Java sprint 1</t>
-  </si>
-  <si>
-    <t>Understand logic</t>
-  </si>
-  <si>
-    <t>MEDIUM</t>
-  </si>
-  <si>
-    <t>2025-07-31</t>
-  </si>
-  <si>
-    <t>f1aa0ec7-7cb9-425a-aea9-63c6ae02f69b</t>
-  </si>
-  <si>
-    <t>Test 5</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>2025-07-22</t>
-  </si>
-  <si>
-    <t>To Do</t>
-  </si>
-  <si>
-    <t>aa303491-34d2-4288-a7de-a1f6447ec458</t>
-  </si>
-  <si>
-    <t>Read and understand the first chapter</t>
-  </si>
-  <si>
     <t>2024-07-31</t>
   </si>
   <si>
@@ -183,22 +195,10 @@
     <t>2025-08-08</t>
   </si>
   <si>
-    <t>b60a251c-299a-4d3d-97bb-7efca4f88f97</t>
-  </si>
-  <si>
-    <t>Coding</t>
-  </si>
-  <si>
-    <t>2025-07-23</t>
-  </si>
-  <si>
     <t>45008821-c270-42fc-9a00-e93c53c9d14c</t>
   </si>
   <si>
     <t>Improve Code</t>
-  </si>
-  <si>
-    <t>HIGH</t>
   </si>
 </sst>
 </file>
@@ -299,21 +299,21 @@
         <v>13</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>18</v>
@@ -363,19 +363,19 @@
         <v>26</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>27</v>
       </c>
       <c r="D2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="F2" t="s" s="0">
         <v>29</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>18</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>30</v>
@@ -389,7 +389,7 @@
         <v>31</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>32</v>
@@ -401,10 +401,10 @@
         <v>34</v>
       </c>
       <c r="F3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s" s="0">
         <v>35</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>30</v>
       </c>
       <c r="H3" t="b" s="0">
         <v>0</v>
@@ -415,7 +415,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>37</v>
@@ -430,7 +430,7 @@
         <v>39</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H4" t="b" s="0">
         <v>0</v>
@@ -438,51 +438,51 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>41</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>42</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>42</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s" s="0">
         <v>43</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="H5" t="b" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s" s="0">
+      <c r="D6" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>46</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>34</v>
       </c>
       <c r="F6" t="s" s="0">
         <v>47</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H6" t="b" s="0">
         <v>1</v>
@@ -490,13 +490,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>50</v>
@@ -508,7 +508,7 @@
         <v>51</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H7" t="b" s="0">
         <v>1</v>
@@ -519,7 +519,7 @@
         <v>52</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>53</v>
@@ -528,13 +528,13 @@
         <v>54</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s" s="0">
         <v>55</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H8" t="b" s="0">
         <v>1</v>
@@ -545,48 +545,48 @@
         <v>56</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>57</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H9" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H10" t="b" s="0">
         <v>0</v>

</xml_diff>

<commit_message>
Implement start day for task
</commit_message>
<xml_diff>
--- a/data/goals_and_tasks.xlsx
+++ b/data/goals_and_tasks.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
   <si>
     <t>Goal ID</t>
   </si>
@@ -27,7 +27,19 @@
     <t>Target Date</t>
   </si>
   <si>
-    <t>127c0a0e-cc50-4e37-bee0-4a4f50c324b8</t>
+    <t>675f64e8-e799-41ad-aded-dc91f1bdd810</t>
+  </si>
+  <si>
+    <t>[August] English Speaking (Elsa)</t>
+  </si>
+  <si>
+    <t>MONTHLY</t>
+  </si>
+  <si>
+    <t>2025-08-31</t>
+  </si>
+  <si>
+    <t>cbdbe564-19b4-42d9-a781-b439e8d3dbba</t>
   </si>
   <si>
     <t>Improve UI Design</t>
@@ -39,7 +51,7 @@
     <t>2025-08-15</t>
   </si>
   <si>
-    <t>309f8b42-1c45-4b11-b939-35e703dbcc92</t>
+    <t>19855b78-d0c4-4113-82ba-dd4058f17eb2</t>
   </si>
   <si>
     <t>Learn Java</t>
@@ -51,7 +63,7 @@
     <t>2024-12-31</t>
   </si>
   <si>
-    <t>b4a0f800-69ca-4f8f-9b02-d7c0ceb3ece0</t>
+    <t>d3822c7e-ed8a-4379-a50a-fa54fd0908fb</t>
   </si>
   <si>
     <t>Learn Spring Boot</t>
@@ -72,6 +84,9 @@
     <t>Task Priority</t>
   </si>
   <si>
+    <t>Task Start Day</t>
+  </si>
+  <si>
     <t>Task Due Date</t>
   </si>
   <si>
@@ -81,6 +96,60 @@
     <t>Task Completed</t>
   </si>
   <si>
+    <t>6bacadb1-60a7-4af1-a87b-abdf913cdf91</t>
+  </si>
+  <si>
+    <t>[Week1] Learning English Speaking</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>2025-08-08</t>
+  </si>
+  <si>
+    <t>2025-08-09</t>
+  </si>
+  <si>
+    <t>To Do</t>
+  </si>
+  <si>
+    <t>757a36bf-83f8-4c68-9d05-b2efdf6174e9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 2] Learning English Speaking </t>
+  </si>
+  <si>
+    <t>2025-08-16</t>
+  </si>
+  <si>
+    <t>184f01f3-6dbc-403d-ba8d-05212f4b3885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 3] Learning English Speaking </t>
+  </si>
+  <si>
+    <t>2025-07-08</t>
+  </si>
+  <si>
+    <t>2025-08-23</t>
+  </si>
+  <si>
+    <t>9ac02799-eb64-4ffc-ba9d-5903b004e511</t>
+  </si>
+  <si>
+    <t>[Week 4] Learning English Speaking</t>
+  </si>
+  <si>
+    <t>2025-08-29</t>
+  </si>
+  <si>
+    <t>2025-08-30</t>
+  </si>
+  <si>
     <t>b60a251c-299a-4d3d-97bb-7efca4f88f97</t>
   </si>
   <si>
@@ -93,7 +162,7 @@
     <t>2025-07-23</t>
   </si>
   <si>
-    <t>To Do</t>
+    <t>2025-07-24</t>
   </si>
   <si>
     <t>5258a021-56cd-4f68-8ef5-386e86136170</t>
@@ -105,60 +174,36 @@
     <t>Improve code 2</t>
   </si>
   <si>
-    <t>MEDIUM</t>
-  </si>
-  <si>
-    <t>2025-07-24</t>
+    <t>2025-07-25</t>
   </si>
   <si>
     <t>In Progress</t>
   </si>
   <si>
-    <t>246b36ce-0da3-49d5-8857-21e915cc6156</t>
-  </si>
-  <si>
-    <t>Learn Java sprint 1</t>
-  </si>
-  <si>
-    <t>Understand logic</t>
-  </si>
-  <si>
-    <t>2025-07-31</t>
-  </si>
-  <si>
     <t>f1aa0ec7-7cb9-425a-aea9-63c6ae02f69b</t>
   </si>
   <si>
     <t>Test 5</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>2025-07-22</t>
   </si>
   <si>
-    <t>aa303491-34d2-4288-a7de-a1f6447ec458</t>
-  </si>
-  <si>
-    <t>Read and understand the first chapter</t>
-  </si>
-  <si>
-    <t>2024-07-31</t>
+    <t>fd6629f6-fa17-4f85-8535-415c81b82152</t>
+  </si>
+  <si>
+    <t>Read and understand the second chapter</t>
+  </si>
+  <si>
+    <t>2024-08-09</t>
+  </si>
+  <si>
+    <t>2024-08-10</t>
   </si>
   <si>
     <t>Done</t>
   </si>
   <si>
-    <t>fd6629f6-fa17-4f85-8535-415c81b82152</t>
-  </si>
-  <si>
-    <t>Read and understand the second chapter</t>
-  </si>
-  <si>
-    <t>2024-08-09</t>
-  </si>
-  <si>
     <t>60253cbd-d36b-42ec-be9b-331b0d225447</t>
   </si>
   <si>
@@ -168,7 +213,7 @@
     <t>Improve code 1</t>
   </si>
   <si>
-    <t>2025-07-08</t>
+    <t>2025-07-09</t>
   </si>
   <si>
     <t>fa838930-1316-42a7-8f8f-28d675abfa9c</t>
@@ -178,9 +223,6 @@
   </si>
   <si>
     <t>Improve code 3</t>
-  </si>
-  <si>
-    <t>2025-08-08</t>
   </si>
   <si>
     <t>45008821-c270-42fc-9a00-e93c53c9d14c</t>
@@ -234,7 +276,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -290,10 +332,24 @@
         <v>13</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>14</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -303,7 +359,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -311,65 +367,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s" s="0">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s" s="0">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="I1" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="H2" t="b" s="0">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I2" t="b" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>29</v>
@@ -378,194 +440,276 @@
         <v>30</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="H3" t="b" s="0">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I3" t="b" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>30</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="H4" t="b" s="0">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I4" t="b" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>30</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="H5" t="b" s="0">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I5" t="b" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="H6" t="b" s="0">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I6" t="b" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s" s="0">
         <v>30</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="H7" t="b" s="0">
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I7" t="b" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s" s="0">
         <v>30</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="H8" t="b" s="0">
-        <v>1</v>
+        <v>48</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I8" t="b" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="H9" t="b" s="0">
+        <v>61</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="I9" t="b" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s" s="0">
         <v>13</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="I10" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E10" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s" s="0">
+      <c r="C11" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="G11" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="H10" t="b" s="0">
+      <c r="H11" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="I11" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I12" t="b" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement GoalView and Statistic right view
</commit_message>
<xml_diff>
--- a/data/goals_and_tasks.xlsx
+++ b/data/goals_and_tasks.xlsx
@@ -27,7 +27,7 @@
     <t>Target Date</t>
   </si>
   <si>
-    <t>675f64e8-e799-41ad-aded-dc91f1bdd810</t>
+    <t>0964ea5a-ea5e-4c45-9787-1479b64fa2ca</t>
   </si>
   <si>
     <t>[August] English Speaking (Elsa)</t>
@@ -39,7 +39,7 @@
     <t>2025-08-31</t>
   </si>
   <si>
-    <t>cbdbe564-19b4-42d9-a781-b439e8d3dbba</t>
+    <t>aa0ec478-ef74-4b20-b014-e9487258c775</t>
   </si>
   <si>
     <t>Improve UI Design</t>
@@ -51,7 +51,7 @@
     <t>2025-08-15</t>
   </si>
   <si>
-    <t>19855b78-d0c4-4113-82ba-dd4058f17eb2</t>
+    <t>b21c8691-eb0f-4674-97fd-78b6d2be89ae</t>
   </si>
   <si>
     <t>Learn Java</t>
@@ -63,7 +63,7 @@
     <t>2024-12-31</t>
   </si>
   <si>
-    <t>d3822c7e-ed8a-4379-a50a-fa54fd0908fb</t>
+    <t>b32b6b14-36d0-492e-9353-e838b3ce8f99</t>
   </si>
   <si>
     <t>Learn Spring Boot</t>
@@ -114,18 +114,21 @@
     <t>2025-08-09</t>
   </si>
   <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>757a36bf-83f8-4c68-9d05-b2efdf6174e9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 2] Learning English Speaking </t>
+  </si>
+  <si>
+    <t>2025-08-16</t>
+  </si>
+  <si>
     <t>To Do</t>
   </si>
   <si>
-    <t>757a36bf-83f8-4c68-9d05-b2efdf6174e9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 2] Learning English Speaking </t>
-  </si>
-  <si>
-    <t>2025-08-16</t>
-  </si>
-  <si>
     <t>184f01f3-6dbc-403d-ba8d-05212f4b3885</t>
   </si>
   <si>
@@ -175,9 +178,6 @@
   </si>
   <si>
     <t>2025-07-25</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>f1aa0ec7-7cb9-425a-aea9-63c6ae02f69b</t>
@@ -446,7 +446,7 @@
         <v>36</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I3" t="b" s="0">
         <v>0</v>
@@ -454,13 +454,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>29</v>
@@ -469,13 +469,13 @@
         <v>30</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I4" t="b" s="0">
         <v>0</v>
@@ -483,13 +483,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>29</v>
@@ -498,13 +498,13 @@
         <v>30</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I5" t="b" s="0">
         <v>0</v>
@@ -512,28 +512,28 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I6" t="b" s="0">
         <v>0</v>
@@ -541,28 +541,28 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>13</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s" s="0">
         <v>30</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="I7" t="b" s="0">
         <v>0</v>
@@ -588,10 +588,10 @@
         <v>57</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I8" t="b" s="0">
         <v>0</v>
@@ -643,7 +643,7 @@
         <v>30</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s" s="0">
         <v>66</v>
@@ -669,7 +669,7 @@
         <v>69</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s" s="0">
         <v>31</v>
@@ -701,16 +701,16 @@
         <v>72</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="I12" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Empty Calendar Right View
</commit_message>
<xml_diff>
--- a/data/goals_and_tasks.xlsx
+++ b/data/goals_and_tasks.xlsx
@@ -27,7 +27,7 @@
     <t>Target Date</t>
   </si>
   <si>
-    <t>0964ea5a-ea5e-4c45-9787-1479b64fa2ca</t>
+    <t>1de00eff-8f4b-4ca0-8f3a-7599e37f2377</t>
   </si>
   <si>
     <t>[August] English Speaking (Elsa)</t>
@@ -39,7 +39,7 @@
     <t>2025-08-31</t>
   </si>
   <si>
-    <t>aa0ec478-ef74-4b20-b014-e9487258c775</t>
+    <t>fd8f018e-252d-4f4f-aea4-254a581b60c3</t>
   </si>
   <si>
     <t>Improve UI Design</t>
@@ -51,7 +51,7 @@
     <t>2025-08-15</t>
   </si>
   <si>
-    <t>b21c8691-eb0f-4674-97fd-78b6d2be89ae</t>
+    <t>f6826d5e-affa-4acb-b0ca-e8df3b0c7119</t>
   </si>
   <si>
     <t>Learn Java</t>
@@ -63,7 +63,7 @@
     <t>2024-12-31</t>
   </si>
   <si>
-    <t>b32b6b14-36d0-492e-9353-e838b3ce8f99</t>
+    <t>7ea47a43-a6c7-4c13-8544-4ca37a998e8c</t>
   </si>
   <si>
     <t>Learn Spring Boot</t>
@@ -105,81 +105,84 @@
     <t/>
   </si>
   <si>
+    <t>URGENT</t>
+  </si>
+  <si>
+    <t>2025-08-08</t>
+  </si>
+  <si>
+    <t>2025-08-09</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>184f01f3-6dbc-403d-ba8d-05212f4b3885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 3] Learning English Speaking </t>
+  </si>
+  <si>
     <t>MEDIUM</t>
   </si>
   <si>
-    <t>2025-08-08</t>
-  </si>
-  <si>
-    <t>2025-08-09</t>
+    <t>2025-07-08</t>
+  </si>
+  <si>
+    <t>2025-08-23</t>
+  </si>
+  <si>
+    <t>To Do</t>
+  </si>
+  <si>
+    <t>9ac02799-eb64-4ffc-ba9d-5903b004e511</t>
+  </si>
+  <si>
+    <t>[Week 4] Learning English Speaking</t>
+  </si>
+  <si>
+    <t>2025-08-29</t>
+  </si>
+  <si>
+    <t>2025-08-30</t>
+  </si>
+  <si>
+    <t>757a36bf-83f8-4c68-9d05-b2efdf6174e9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 2] Learning English Speaking </t>
+  </si>
+  <si>
+    <t>2025-08-16</t>
+  </si>
+  <si>
+    <t>b60a251c-299a-4d3d-97bb-7efca4f88f97</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>2025-07-23</t>
+  </si>
+  <si>
+    <t>2025-07-24</t>
+  </si>
+  <si>
+    <t>5258a021-56cd-4f68-8ef5-386e86136170</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Improve code 2</t>
+  </si>
+  <si>
+    <t>2025-07-25</t>
   </si>
   <si>
     <t>In Progress</t>
   </si>
   <si>
-    <t>757a36bf-83f8-4c68-9d05-b2efdf6174e9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 2] Learning English Speaking </t>
-  </si>
-  <si>
-    <t>2025-08-16</t>
-  </si>
-  <si>
-    <t>To Do</t>
-  </si>
-  <si>
-    <t>184f01f3-6dbc-403d-ba8d-05212f4b3885</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 3] Learning English Speaking </t>
-  </si>
-  <si>
-    <t>2025-07-08</t>
-  </si>
-  <si>
-    <t>2025-08-23</t>
-  </si>
-  <si>
-    <t>9ac02799-eb64-4ffc-ba9d-5903b004e511</t>
-  </si>
-  <si>
-    <t>[Week 4] Learning English Speaking</t>
-  </si>
-  <si>
-    <t>2025-08-29</t>
-  </si>
-  <si>
-    <t>2025-08-30</t>
-  </si>
-  <si>
-    <t>b60a251c-299a-4d3d-97bb-7efca4f88f97</t>
-  </si>
-  <si>
-    <t>Coding</t>
-  </si>
-  <si>
-    <t>URGENT</t>
-  </si>
-  <si>
-    <t>2025-07-23</t>
-  </si>
-  <si>
-    <t>2025-07-24</t>
-  </si>
-  <si>
-    <t>5258a021-56cd-4f68-8ef5-386e86136170</t>
-  </si>
-  <si>
-    <t>Test 2</t>
-  </si>
-  <si>
-    <t>Improve code 2</t>
-  </si>
-  <si>
-    <t>2025-07-25</t>
-  </si>
-  <si>
     <t>f1aa0ec7-7cb9-425a-aea9-63c6ae02f69b</t>
   </si>
   <si>
@@ -199,9 +202,6 @@
   </si>
   <si>
     <t>2024-08-10</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t>60253cbd-d36b-42ec-be9b-331b0d225447</t>
@@ -420,7 +420,7 @@
         <v>33</v>
       </c>
       <c r="I2" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -437,16 +437,16 @@
         <v>29</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I3" t="b" s="0">
         <v>0</v>
@@ -454,28 +454,28 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>29</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I4" t="b" s="0">
         <v>0</v>
@@ -483,48 +483,48 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>29</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I5" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s" s="0">
         <v>49</v>
@@ -533,7 +533,7 @@
         <v>50</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I6" t="b" s="0">
         <v>0</v>
@@ -553,7 +553,7 @@
         <v>53</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s" s="0">
         <v>50</v>
@@ -562,7 +562,7 @@
         <v>54</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I7" t="b" s="0">
         <v>0</v>
@@ -570,28 +570,28 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s" s="0">
         <v>13</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s" s="0">
         <v>29</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G8" t="s" s="0">
         <v>49</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I8" t="b" s="0">
         <v>0</v>
@@ -599,28 +599,28 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s" s="0">
         <v>13</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="I9" t="b" s="0">
         <v>1</v>
@@ -640,16 +640,16 @@
         <v>65</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s" s="0">
         <v>66</v>
       </c>
       <c r="H10" t="s" s="0">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="I10" t="b" s="0">
         <v>1</v>
@@ -669,7 +669,7 @@
         <v>69</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s" s="0">
         <v>31</v>
@@ -678,7 +678,7 @@
         <v>32</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="I11" t="b" s="0">
         <v>1</v>
@@ -707,7 +707,7 @@
         <v>50</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="I12" t="b" s="0">
         <v>1</v>

</xml_diff>